<commit_message>
* Add text box.
</commit_message>
<xml_diff>
--- a/doc/TimeSavingBox.xlsx
+++ b/doc/TimeSavingBox.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\develop\work\AndroidStudioProjects\TimeSavingBox\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A1290D-03AC-4AB4-B198-BBA5321E79B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FC510E5-D5D3-4F74-96BB-AAFBD731F485}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-50" yWindow="30" windowWidth="23040" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="プロダクトバックログ" sheetId="3" r:id="rId1"/>
@@ -19,9 +19,9 @@
     <sheet name="dummy" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">プロダクトバックログ!$A$1:$V$27</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">プロダクトバックログ!$A$1:$V$31</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="106">
   <si>
     <t>■dummy</t>
     <phoneticPr fontId="1"/>
@@ -281,16 +281,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>[保存]したことがわかるメッセージが表示される</t>
-    <rPh sb="1" eb="3">
-      <t>ホゾン</t>
-    </rPh>
-    <rPh sb="18" eb="20">
-      <t>ヒョウジ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>[開始日時]入力のテキストボックスがある</t>
     <rPh sb="1" eb="3">
       <t>カイシ</t>
@@ -733,6 +723,50 @@
   </si>
   <si>
     <t>タスク</t>
+  </si>
+  <si>
+    <t>画面表示</t>
+    <rPh sb="0" eb="2">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ソースコード</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Androidのメッセージ表示の実装方法を理解していること</t>
+    <rPh sb="13" eb="15">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>ジッソウ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>ホウホウ</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>リカイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[保存]したことがわかるメッセージが画面に表示される
+(Toastではない)</t>
+    <rPh sb="1" eb="3">
+      <t>ホゾン</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -1426,27 +1460,32 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:Z27"/>
+  <dimension ref="A2:Z31"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A8" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="U21" sqref="U21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" outlineLevelRow="1" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="2.58203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="4.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.58203125" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="28.08203125" style="2" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="25.58203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="28.08203125" style="2" customWidth="1" outlineLevel="1"/>
     <col min="5" max="5" width="25.58203125" style="2" customWidth="1"/>
     <col min="6" max="8" width="8.6640625" style="1"/>
     <col min="9" max="10" width="25.58203125" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="8.6640625" style="1"/>
+    <col min="11" max="16" width="8.6640625" style="1"/>
+    <col min="17" max="18" width="8.6640625" style="3"/>
+    <col min="19" max="19" width="8.6640625" style="1"/>
+    <col min="20" max="20" width="12.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:2">
       <c r="B2" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="2:2">
@@ -1493,7 +1532,7 @@
         <v>10</v>
       </c>
       <c r="N18" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O18" s="6" t="s">
         <v>11</v>
@@ -1501,10 +1540,10 @@
       <c r="P18" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="Q18" s="6" t="s">
+      <c r="Q18" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="R18" s="6" t="s">
+      <c r="R18" s="7" t="s">
         <v>14</v>
       </c>
       <c r="S18" s="6" t="s">
@@ -1554,8 +1593,8 @@
       <c r="N19" s="9"/>
       <c r="O19" s="9"/>
       <c r="P19" s="9"/>
-      <c r="Q19" s="9"/>
-      <c r="R19" s="9"/>
+      <c r="Q19" s="8"/>
+      <c r="R19" s="8"/>
       <c r="S19" s="9"/>
       <c r="T19" s="9"/>
       <c r="U19" s="9"/>
@@ -1566,38 +1605,34 @@
         <v>1</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>39</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="E20" s="6"/>
       <c r="F20" s="9"/>
-      <c r="G20" s="9" t="s">
-        <v>32</v>
-      </c>
+      <c r="G20" s="9"/>
       <c r="H20" s="9"/>
-      <c r="I20" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="J20" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="K20" s="9" t="s">
-        <v>102</v>
-      </c>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="9"/>
       <c r="L20" s="9"/>
       <c r="M20" s="9"/>
       <c r="N20" s="9"/>
       <c r="O20" s="9"/>
       <c r="P20" s="9"/>
-      <c r="Q20" s="9"/>
-      <c r="R20" s="9"/>
+      <c r="Q20" s="8">
+        <v>1</v>
+      </c>
+      <c r="R20" s="8"/>
       <c r="S20" s="9"/>
-      <c r="T20" s="9"/>
-      <c r="U20" s="9"/>
+      <c r="T20" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="U20" s="9" t="s">
+        <v>102</v>
+      </c>
       <c r="V20" s="9"/>
     </row>
     <row r="21" spans="1:26" ht="36">
@@ -1605,25 +1640,29 @@
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F21" s="9"/>
       <c r="G21" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H21" s="9"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
+      <c r="I21" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="K21" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L21" s="9"/>
       <c r="M21" s="9"/>
       <c r="N21" s="9"/>
       <c r="O21" s="9"/>
       <c r="P21" s="9"/>
-      <c r="Q21" s="9"/>
-      <c r="R21" s="9"/>
+      <c r="Q21" s="8"/>
+      <c r="R21" s="8"/>
       <c r="S21" s="9"/>
       <c r="T21" s="9"/>
       <c r="U21" s="9"/>
@@ -1634,25 +1673,25 @@
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F22" s="9"/>
       <c r="G22" s="9" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="H22" s="9"/>
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
       <c r="K22" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L22" s="9"/>
       <c r="M22" s="9"/>
       <c r="N22" s="9"/>
       <c r="O22" s="9"/>
       <c r="P22" s="9"/>
-      <c r="Q22" s="9"/>
-      <c r="R22" s="9"/>
+      <c r="Q22" s="8"/>
+      <c r="R22" s="8"/>
       <c r="S22" s="9"/>
       <c r="T22" s="9"/>
       <c r="U22" s="9"/>
@@ -1663,167 +1702,282 @@
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F23" s="9"/>
       <c r="G23" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H23" s="9"/>
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
       <c r="K23" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L23" s="9"/>
       <c r="M23" s="9"/>
       <c r="N23" s="9"/>
       <c r="O23" s="9"/>
       <c r="P23" s="9"/>
-      <c r="Q23" s="9"/>
-      <c r="R23" s="9"/>
+      <c r="Q23" s="8"/>
+      <c r="R23" s="8"/>
       <c r="S23" s="9"/>
       <c r="T23" s="9"/>
       <c r="U23" s="9"/>
       <c r="V23" s="9"/>
     </row>
     <row r="24" spans="1:26" ht="36">
-      <c r="B24" s="8">
-        <v>2</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>50</v>
-      </c>
+      <c r="B24" s="8"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
       <c r="E24" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F24" s="9"/>
       <c r="G24" s="9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H24" s="9"/>
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
       <c r="K24" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L24" s="9"/>
       <c r="M24" s="9"/>
       <c r="N24" s="9"/>
       <c r="O24" s="9"/>
       <c r="P24" s="9"/>
-      <c r="Q24" s="9"/>
-      <c r="R24" s="9"/>
+      <c r="Q24" s="8"/>
+      <c r="R24" s="8"/>
       <c r="S24" s="9"/>
       <c r="T24" s="9"/>
       <c r="U24" s="9"/>
       <c r="V24" s="9"/>
     </row>
     <row r="25" spans="1:26" ht="36">
-      <c r="B25" s="8"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6" t="s">
-        <v>38</v>
-      </c>
+      <c r="B25" s="8">
+        <v>2</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E25" s="6"/>
       <c r="F25" s="9"/>
-      <c r="G25" s="9" t="s">
-        <v>48</v>
-      </c>
+      <c r="G25" s="9"/>
       <c r="H25" s="9"/>
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
-      <c r="K25" s="9" t="s">
-        <v>102</v>
-      </c>
+      <c r="K25" s="9"/>
       <c r="L25" s="9"/>
       <c r="M25" s="9"/>
       <c r="N25" s="9"/>
       <c r="O25" s="9"/>
       <c r="P25" s="9"/>
-      <c r="Q25" s="9"/>
-      <c r="R25" s="9"/>
+      <c r="Q25" s="8">
+        <f>SUM(R26:R27)</f>
+        <v>3</v>
+      </c>
+      <c r="R25" s="8"/>
       <c r="S25" s="9"/>
-      <c r="T25" s="9"/>
-      <c r="U25" s="9"/>
+      <c r="T25" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="U25" s="9" t="s">
+        <v>102</v>
+      </c>
       <c r="V25" s="9"/>
     </row>
-    <row r="26" spans="1:26" ht="72">
-      <c r="B26" s="8">
-        <v>3</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>47</v>
-      </c>
+    <row r="26" spans="1:26" ht="36">
+      <c r="B26" s="8"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
       <c r="E26" s="6" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
+      <c r="G26" s="9" t="s">
+        <v>34</v>
+      </c>
       <c r="H26" s="9"/>
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
       <c r="K26" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L26" s="9"/>
       <c r="M26" s="9"/>
       <c r="N26" s="9"/>
       <c r="O26" s="9"/>
       <c r="P26" s="9"/>
-      <c r="Q26" s="9"/>
-      <c r="R26" s="9"/>
+      <c r="Q26" s="8"/>
+      <c r="R26" s="8">
+        <v>1</v>
+      </c>
       <c r="S26" s="9"/>
       <c r="T26" s="9"/>
       <c r="U26" s="9"/>
       <c r="V26" s="9"/>
     </row>
     <row r="27" spans="1:26" ht="54">
-      <c r="B27" s="8">
-        <v>4</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>49</v>
-      </c>
+      <c r="B27" s="8"/>
+      <c r="C27" s="6"/>
       <c r="D27" s="6"/>
       <c r="E27" s="6" t="s">
-        <v>41</v>
+        <v>105</v>
       </c>
       <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
+      <c r="G27" s="9" t="s">
+        <v>47</v>
+      </c>
       <c r="H27" s="9"/>
-      <c r="I27" s="6"/>
+      <c r="I27" s="6" t="s">
+        <v>104</v>
+      </c>
       <c r="J27" s="6"/>
       <c r="K27" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L27" s="9"/>
       <c r="M27" s="9"/>
       <c r="N27" s="9"/>
       <c r="O27" s="9"/>
       <c r="P27" s="9"/>
-      <c r="Q27" s="9"/>
-      <c r="R27" s="9"/>
+      <c r="Q27" s="8"/>
+      <c r="R27" s="8">
+        <v>2</v>
+      </c>
       <c r="S27" s="9"/>
       <c r="T27" s="9"/>
       <c r="U27" s="9"/>
       <c r="V27" s="9"/>
     </row>
+    <row r="28" spans="1:26" ht="72">
+      <c r="B28" s="8">
+        <v>3</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="9"/>
+      <c r="P28" s="9"/>
+      <c r="Q28" s="8"/>
+      <c r="R28" s="8"/>
+      <c r="S28" s="9"/>
+      <c r="T28" s="9"/>
+      <c r="U28" s="9"/>
+      <c r="V28" s="9"/>
+    </row>
+    <row r="29" spans="1:26" ht="54">
+      <c r="B29" s="8"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="L29" s="9"/>
+      <c r="M29" s="9"/>
+      <c r="N29" s="9"/>
+      <c r="O29" s="9"/>
+      <c r="P29" s="9"/>
+      <c r="Q29" s="8"/>
+      <c r="R29" s="8"/>
+      <c r="S29" s="9"/>
+      <c r="T29" s="9"/>
+      <c r="U29" s="9"/>
+      <c r="V29" s="9"/>
+    </row>
+    <row r="30" spans="1:26" ht="54">
+      <c r="B30" s="8">
+        <v>4</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9"/>
+      <c r="N30" s="9"/>
+      <c r="O30" s="9"/>
+      <c r="P30" s="9"/>
+      <c r="Q30" s="8"/>
+      <c r="R30" s="8"/>
+      <c r="S30" s="9"/>
+      <c r="T30" s="9"/>
+      <c r="U30" s="9"/>
+      <c r="V30" s="9"/>
+    </row>
+    <row r="31" spans="1:26" ht="54">
+      <c r="B31" s="8"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="L31" s="9"/>
+      <c r="M31" s="9"/>
+      <c r="N31" s="9"/>
+      <c r="O31" s="9"/>
+      <c r="P31" s="9"/>
+      <c r="Q31" s="8"/>
+      <c r="R31" s="8"/>
+      <c r="S31" s="9"/>
+      <c r="T31" s="9"/>
+      <c r="U31" s="9"/>
+      <c r="V31" s="9"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K20:K27" xr:uid="{28DE5D51-C321-4870-B1C8-48B479072D32}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K20:K31" xr:uid="{28DE5D51-C321-4870-B1C8-48B479072D32}">
       <formula1>"タスク,税,Spike,前提条件(技術的負債)"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="50" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="44" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;F　&amp;A&amp;R&amp;D　&amp;T</oddHeader>
     <oddFooter>&amp;C&amp;P</oddFooter>
@@ -1849,17 +2003,17 @@
   <sheetData>
     <row r="2" spans="2:4">
       <c r="B2" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="2:4">
       <c r="B3" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="2:4">
       <c r="B4" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="2:4">
@@ -1867,7 +2021,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D6" s="5"/>
     </row>
@@ -1876,7 +2030,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D7" s="5"/>
     </row>
@@ -1885,7 +2039,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D8" s="5"/>
     </row>
@@ -1894,7 +2048,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D9" s="5"/>
     </row>
@@ -1903,88 +2057,88 @@
         <v>5</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D10" s="5"/>
     </row>
     <row r="11" spans="2:4">
       <c r="C11" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>71</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="12" spans="2:4">
       <c r="C12" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>73</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="13" spans="2:4">
       <c r="C13" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>75</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="14" spans="2:4">
       <c r="C14" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>77</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="15" spans="2:4">
       <c r="C15" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>79</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="16" spans="2:4">
       <c r="C16" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>81</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="17" spans="2:4">
       <c r="C17" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>83</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="18" spans="2:4">
       <c r="C18" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>85</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="19" spans="2:4">
       <c r="C19" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="20" spans="2:4">
       <c r="C20" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>89</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="21" spans="2:4">
@@ -1992,7 +2146,7 @@
         <v>6</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D21" s="5"/>
     </row>
@@ -2001,7 +2155,7 @@
         <v>7</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D22" s="5"/>
     </row>
@@ -2010,23 +2164,23 @@
         <v>10</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="2:4">
       <c r="C25" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="2:4">
       <c r="C26" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="2:4">
@@ -2034,23 +2188,23 @@
         <v>11</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="2:4">
       <c r="C28" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="29" spans="2:4">
       <c r="C29" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="30" spans="2:4">
@@ -2058,23 +2212,23 @@
         <v>12</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="31" spans="2:4">
       <c r="C31" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="32" spans="2:4">
       <c r="C32" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2116,36 +2270,36 @@
     </row>
     <row r="12" spans="2:12">
       <c r="I12" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="2:12">
       <c r="I14" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J14" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L14" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="15" spans="2:12">
       <c r="I15" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="2:12">
       <c r="I16" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="9:10">
       <c r="I18" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* Save starttime and endtime.
</commit_message>
<xml_diff>
--- a/doc/TimeSavingBox.xlsx
+++ b/doc/TimeSavingBox.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\develop\work\AndroidStudioProjects\TimeSavingBox\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FC510E5-D5D3-4F74-96BB-AAFBD731F485}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57B027F7-2116-4C93-BDA4-4D341D3054BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-50" yWindow="30" windowWidth="23040" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34440" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="プロダクトバックログ" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="dummy" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">プロダクトバックログ!$A$1:$V$31</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">プロダクトバックログ!$A$1:$W$31</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="108">
   <si>
     <t>■dummy</t>
     <phoneticPr fontId="1"/>
@@ -360,25 +360,6 @@
     </rPh>
     <rPh sb="35" eb="37">
       <t>カクニン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>利用者は[開始日時][終了日時][メモ]を1つ保存できる</t>
-    <rPh sb="0" eb="3">
-      <t>リヨウシャ</t>
-    </rPh>
-    <rPh sb="5" eb="7">
-      <t>カイシ</t>
-    </rPh>
-    <rPh sb="7" eb="9">
-      <t>ニチジ</t>
-    </rPh>
-    <rPh sb="11" eb="13">
-      <t>シュウリョウ</t>
-    </rPh>
-    <rPh sb="23" eb="25">
-      <t>ホゾン</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -765,6 +746,69 @@
     </rPh>
     <rPh sb="21" eb="23">
       <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DBにデータが保存されていることを確認できること</t>
+    <rPh sb="7" eb="9">
+      <t>ホゾン</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>カクニン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>利用者は[開始日時][終了日時][メモ]を</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1つ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>保存できる</t>
+    </r>
+    <rPh sb="0" eb="3">
+      <t>リヨウシャ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>カイシ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>ニチジ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>シュウリョウ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>ホゾン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>実績工数</t>
+    <rPh sb="0" eb="2">
+      <t>ジッセキ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>コウスウ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -773,7 +817,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -794,6 +838,15 @@
       <color theme="1"/>
       <name val="Yu Gothic"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Yu Gothic"/>
+      <family val="3"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1155,16 +1208,16 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>298000</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>170487</xdr:rowOff>
+      <xdr:colOff>105938</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>149902</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="図 4">
+        <xdr:cNvPr id="2" name="図 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D815233-5E0F-4FB0-849F-EC6EB36F1C1A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A637BA2B-3A0E-4FFE-8ED1-558E40F6AB30}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1180,8 +1233,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="658813" y="1150938"/>
-          <a:ext cx="3592062" cy="7766674"/>
+          <a:off x="198438" y="1150938"/>
+          <a:ext cx="3400000" cy="7285714"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1460,10 +1513,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:Z31"/>
+  <dimension ref="A2:AA31"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A8" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="U21" sqref="U21"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A14" zoomScale="80" zoomScaleNormal="60" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="T25" sqref="T25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -1476,16 +1529,16 @@
     <col min="6" max="8" width="8.6640625" style="1"/>
     <col min="9" max="10" width="25.58203125" style="2" customWidth="1"/>
     <col min="11" max="16" width="8.6640625" style="1"/>
-    <col min="17" max="18" width="8.6640625" style="3"/>
-    <col min="19" max="19" width="8.6640625" style="1"/>
-    <col min="20" max="20" width="12.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="8.6640625" style="1"/>
+    <col min="17" max="19" width="8.6640625" style="3"/>
+    <col min="20" max="20" width="8.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:2">
       <c r="B2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="2:2">
@@ -1493,7 +1546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:26" s="2" customFormat="1" ht="36" collapsed="1">
+    <row r="18" spans="1:27" s="2" customFormat="1" ht="36" collapsed="1">
       <c r="A18" s="10"/>
       <c r="B18" s="7" t="s">
         <v>3</v>
@@ -1532,7 +1585,7 @@
         <v>10</v>
       </c>
       <c r="N18" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O18" s="6" t="s">
         <v>11</v>
@@ -1546,32 +1599,35 @@
       <c r="R18" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="S18" s="6" t="s">
+      <c r="S18" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="T18" s="6" t="s">
+      <c r="T18" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="U18" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="U18" s="6" t="s">
+      <c r="V18" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="V18" s="6" t="s">
+      <c r="W18" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="W18" s="2" t="s">
+      <c r="X18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="X18" s="2" t="s">
+      <c r="Y18" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="Y18" s="2" t="s">
+      <c r="Z18" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="Z18" s="2" t="s">
+      <c r="AA18" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:26" hidden="1" outlineLevel="1">
+    <row r="19" spans="1:27" hidden="1" outlineLevel="1">
       <c r="B19" s="8"/>
       <c r="C19" s="6" t="s">
         <v>27</v>
@@ -1595,12 +1651,13 @@
       <c r="P19" s="9"/>
       <c r="Q19" s="8"/>
       <c r="R19" s="8"/>
-      <c r="S19" s="9"/>
-      <c r="T19" s="9"/>
+      <c r="S19" s="8"/>
+      <c r="T19" s="8"/>
       <c r="U19" s="9"/>
       <c r="V19" s="9"/>
-    </row>
-    <row r="20" spans="1:26" ht="54">
+      <c r="W19" s="9"/>
+    </row>
+    <row r="20" spans="1:27" ht="54">
       <c r="B20" s="8">
         <v>1</v>
       </c>
@@ -1608,15 +1665,21 @@
         <v>42</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
       <c r="H20" s="9"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="9"/>
+      <c r="I20" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="K20" s="9" t="s">
+        <v>100</v>
+      </c>
       <c r="L20" s="9"/>
       <c r="M20" s="9"/>
       <c r="N20" s="9"/>
@@ -1626,16 +1689,19 @@
         <v>1</v>
       </c>
       <c r="R20" s="8"/>
-      <c r="S20" s="9"/>
-      <c r="T20" s="9" t="s">
-        <v>103</v>
+      <c r="S20" s="8"/>
+      <c r="T20" s="8">
+        <v>1</v>
       </c>
       <c r="U20" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="V20" s="9"/>
-    </row>
-    <row r="21" spans="1:26" ht="36">
+      <c r="V20" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="W20" s="9"/>
+    </row>
+    <row r="21" spans="1:27" ht="36">
       <c r="B21" s="8"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
@@ -1647,14 +1713,10 @@
         <v>32</v>
       </c>
       <c r="H21" s="9"/>
-      <c r="I21" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="J21" s="6" t="s">
-        <v>61</v>
-      </c>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
       <c r="K21" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L21" s="9"/>
       <c r="M21" s="9"/>
@@ -1663,12 +1725,13 @@
       <c r="P21" s="9"/>
       <c r="Q21" s="8"/>
       <c r="R21" s="8"/>
-      <c r="S21" s="9"/>
-      <c r="T21" s="9"/>
+      <c r="S21" s="8"/>
+      <c r="T21" s="8"/>
       <c r="U21" s="9"/>
       <c r="V21" s="9"/>
-    </row>
-    <row r="22" spans="1:26" ht="36">
+      <c r="W21" s="9"/>
+    </row>
+    <row r="22" spans="1:27" ht="36">
       <c r="B22" s="8"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
@@ -1683,7 +1746,7 @@
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
       <c r="K22" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L22" s="9"/>
       <c r="M22" s="9"/>
@@ -1692,12 +1755,13 @@
       <c r="P22" s="9"/>
       <c r="Q22" s="8"/>
       <c r="R22" s="8"/>
-      <c r="S22" s="9"/>
-      <c r="T22" s="9"/>
+      <c r="S22" s="8"/>
+      <c r="T22" s="8"/>
       <c r="U22" s="9"/>
       <c r="V22" s="9"/>
-    </row>
-    <row r="23" spans="1:26" ht="36">
+      <c r="W22" s="9"/>
+    </row>
+    <row r="23" spans="1:27" ht="36">
       <c r="B23" s="8"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
@@ -1712,7 +1776,7 @@
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
       <c r="K23" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L23" s="9"/>
       <c r="M23" s="9"/>
@@ -1721,12 +1785,13 @@
       <c r="P23" s="9"/>
       <c r="Q23" s="8"/>
       <c r="R23" s="8"/>
-      <c r="S23" s="9"/>
-      <c r="T23" s="9"/>
+      <c r="S23" s="8"/>
+      <c r="T23" s="8"/>
       <c r="U23" s="9"/>
       <c r="V23" s="9"/>
-    </row>
-    <row r="24" spans="1:26" ht="36">
+      <c r="W23" s="9"/>
+    </row>
+    <row r="24" spans="1:27" ht="36">
       <c r="B24" s="8"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -1741,7 +1806,7 @@
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
       <c r="K24" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L24" s="9"/>
       <c r="M24" s="9"/>
@@ -1750,27 +1815,30 @@
       <c r="P24" s="9"/>
       <c r="Q24" s="8"/>
       <c r="R24" s="8"/>
-      <c r="S24" s="9"/>
-      <c r="T24" s="9"/>
+      <c r="S24" s="8"/>
+      <c r="T24" s="8"/>
       <c r="U24" s="9"/>
       <c r="V24" s="9"/>
-    </row>
-    <row r="25" spans="1:26" ht="36">
+      <c r="W24" s="9"/>
+    </row>
+    <row r="25" spans="1:27" ht="36">
       <c r="B25" s="8">
         <v>2</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>43</v>
+        <v>106</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
       <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
+      <c r="J25" s="6" t="s">
+        <v>105</v>
+      </c>
       <c r="K25" s="9"/>
       <c r="L25" s="9"/>
       <c r="M25" s="9"/>
@@ -1782,16 +1850,17 @@
         <v>3</v>
       </c>
       <c r="R25" s="8"/>
-      <c r="S25" s="9"/>
-      <c r="T25" s="9" t="s">
-        <v>103</v>
-      </c>
+      <c r="S25" s="8"/>
+      <c r="T25" s="8"/>
       <c r="U25" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="V25" s="9"/>
-    </row>
-    <row r="26" spans="1:26" ht="36">
+      <c r="V25" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="W25" s="9"/>
+    </row>
+    <row r="26" spans="1:27" ht="36">
       <c r="B26" s="8"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
@@ -1806,7 +1875,7 @@
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
       <c r="K26" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L26" s="9"/>
       <c r="M26" s="9"/>
@@ -1817,29 +1886,32 @@
       <c r="R26" s="8">
         <v>1</v>
       </c>
-      <c r="S26" s="9"/>
-      <c r="T26" s="9"/>
+      <c r="S26" s="8"/>
+      <c r="T26" s="8">
+        <v>1</v>
+      </c>
       <c r="U26" s="9"/>
       <c r="V26" s="9"/>
-    </row>
-    <row r="27" spans="1:26" ht="54">
+      <c r="W26" s="9"/>
+    </row>
+    <row r="27" spans="1:27" ht="54">
       <c r="B27" s="8"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
       <c r="E27" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F27" s="9"/>
       <c r="G27" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H27" s="9"/>
       <c r="I27" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J27" s="6"/>
       <c r="K27" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L27" s="9"/>
       <c r="M27" s="9"/>
@@ -1850,20 +1922,21 @@
       <c r="R27" s="8">
         <v>2</v>
       </c>
-      <c r="S27" s="9"/>
-      <c r="T27" s="9"/>
+      <c r="S27" s="8"/>
+      <c r="T27" s="8"/>
       <c r="U27" s="9"/>
       <c r="V27" s="9"/>
-    </row>
-    <row r="28" spans="1:26" ht="72">
+      <c r="W27" s="9"/>
+    </row>
+    <row r="28" spans="1:27" ht="72">
       <c r="B28" s="8">
         <v>3</v>
       </c>
       <c r="C28" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D28" s="6" t="s">
         <v>45</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>46</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>41</v>
@@ -1881,12 +1954,13 @@
       <c r="P28" s="9"/>
       <c r="Q28" s="8"/>
       <c r="R28" s="8"/>
-      <c r="S28" s="9"/>
-      <c r="T28" s="9"/>
+      <c r="S28" s="8"/>
+      <c r="T28" s="8"/>
       <c r="U28" s="9"/>
       <c r="V28" s="9"/>
-    </row>
-    <row r="29" spans="1:26" ht="54">
+      <c r="W28" s="9"/>
+    </row>
+    <row r="29" spans="1:27" ht="54">
       <c r="B29" s="8"/>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
@@ -1899,7 +1973,7 @@
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
       <c r="K29" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L29" s="9"/>
       <c r="M29" s="9"/>
@@ -1908,17 +1982,18 @@
       <c r="P29" s="9"/>
       <c r="Q29" s="8"/>
       <c r="R29" s="8"/>
-      <c r="S29" s="9"/>
-      <c r="T29" s="9"/>
+      <c r="S29" s="8"/>
+      <c r="T29" s="8"/>
       <c r="U29" s="9"/>
       <c r="V29" s="9"/>
-    </row>
-    <row r="30" spans="1:26" ht="54">
+      <c r="W29" s="9"/>
+    </row>
+    <row r="30" spans="1:27" ht="54">
       <c r="B30" s="8">
         <v>4</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
@@ -1928,7 +2003,7 @@
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
       <c r="K30" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L30" s="9"/>
       <c r="M30" s="9"/>
@@ -1937,12 +2012,13 @@
       <c r="P30" s="9"/>
       <c r="Q30" s="8"/>
       <c r="R30" s="8"/>
-      <c r="S30" s="9"/>
-      <c r="T30" s="9"/>
+      <c r="S30" s="8"/>
+      <c r="T30" s="8"/>
       <c r="U30" s="9"/>
       <c r="V30" s="9"/>
-    </row>
-    <row r="31" spans="1:26" ht="54">
+      <c r="W30" s="9"/>
+    </row>
+    <row r="31" spans="1:27" ht="54">
       <c r="B31" s="8"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
@@ -1955,7 +2031,7 @@
       <c r="I31" s="6"/>
       <c r="J31" s="6"/>
       <c r="K31" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L31" s="9"/>
       <c r="M31" s="9"/>
@@ -1964,20 +2040,21 @@
       <c r="P31" s="9"/>
       <c r="Q31" s="8"/>
       <c r="R31" s="8"/>
-      <c r="S31" s="9"/>
-      <c r="T31" s="9"/>
+      <c r="S31" s="8"/>
+      <c r="T31" s="8"/>
       <c r="U31" s="9"/>
       <c r="V31" s="9"/>
+      <c r="W31" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K20:K31" xr:uid="{28DE5D51-C321-4870-B1C8-48B479072D32}">
       <formula1>"タスク,税,Spike,前提条件(技術的負債)"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="44" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="43" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;F　&amp;A&amp;R&amp;D　&amp;T</oddHeader>
     <oddFooter>&amp;C&amp;P</oddFooter>
@@ -2003,17 +2080,17 @@
   <sheetData>
     <row r="2" spans="2:4">
       <c r="B2" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="2:4">
       <c r="B3" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="2:4">
       <c r="B4" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="2:4">
@@ -2021,7 +2098,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D6" s="5"/>
     </row>
@@ -2030,7 +2107,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D7" s="5"/>
     </row>
@@ -2039,7 +2116,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D8" s="5"/>
     </row>
@@ -2048,7 +2125,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D9" s="5"/>
     </row>
@@ -2057,88 +2134,88 @@
         <v>5</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D10" s="5"/>
     </row>
     <row r="11" spans="2:4">
       <c r="C11" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="12" spans="2:4">
       <c r="C12" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>72</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="13" spans="2:4">
       <c r="C13" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>74</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="14" spans="2:4">
       <c r="C14" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>76</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="15" spans="2:4">
       <c r="C15" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>78</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="16" spans="2:4">
       <c r="C16" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>80</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="17" spans="2:4">
       <c r="C17" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>82</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="18" spans="2:4">
       <c r="C18" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>84</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="19" spans="2:4">
       <c r="C19" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>86</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="20" spans="2:4">
       <c r="C20" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>88</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="21" spans="2:4">
@@ -2146,7 +2223,7 @@
         <v>6</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D21" s="5"/>
     </row>
@@ -2155,7 +2232,7 @@
         <v>7</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D22" s="5"/>
     </row>
@@ -2164,23 +2241,23 @@
         <v>10</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="2:4">
       <c r="C25" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="2:4">
       <c r="C26" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="2:4">
@@ -2188,23 +2265,23 @@
         <v>11</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="2:4">
       <c r="C28" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="2:4">
       <c r="C29" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="30" spans="2:4">
@@ -2212,23 +2289,23 @@
         <v>12</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="2:4">
       <c r="C31" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="2:4">
       <c r="C32" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -2244,10 +2321,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09363CDA-215F-4EDD-B056-6F8D39E04988}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="B2:L18"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -2270,42 +2350,42 @@
     </row>
     <row r="12" spans="2:12">
       <c r="I12" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="2:12">
       <c r="I14" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L14" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="15" spans="2:12">
       <c r="I15" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="2:12">
       <c r="I16" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="9:10">
       <c r="I18" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="80" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;F　&amp;A&amp;R&amp;D　&amp;T</oddHeader>
     <oddFooter>&amp;C&amp;P</oddFooter>

</xml_diff>

<commit_message>
* Add new button.
</commit_message>
<xml_diff>
--- a/doc/TimeSavingBox.xlsx
+++ b/doc/TimeSavingBox.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\develop\work\AndroidStudioProjects\TimeSavingBox\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57B027F7-2116-4C93-BDA4-4D341D3054BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D6A66B-249A-4295-95F8-4EF8BA0E987A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34440" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36300" yWindow="690" windowWidth="23040" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="プロダクトバックログ" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="dummy" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">プロダクトバックログ!$A$1:$W$31</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">プロダクトバックログ!$A$1:$X$34</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="117">
   <si>
     <t>■dummy</t>
     <phoneticPr fontId="1"/>
@@ -111,16 +111,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>見積(相対)</t>
-    <rPh sb="0" eb="2">
-      <t>ミツモリ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>ソウタイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>当初予定(絶対)</t>
     <rPh sb="0" eb="4">
       <t>トウショヨテイ</t>
@@ -537,13 +527,6 @@
   </si>
   <si>
     <t>Now</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>テスト実装</t>
-    <rPh sb="3" eb="5">
-      <t>ジッソウ</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -809,6 +792,151 @@
     </rPh>
     <rPh sb="2" eb="4">
       <t>コウスウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>数値の入力時間を短縮したいから</t>
+    <rPh sb="0" eb="2">
+      <t>スウチ</t>
+    </rPh>
+    <rPh sb="3" eb="7">
+      <t>ニュウリョクジカン</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>タンシュク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>完了日</t>
+    <rPh sb="0" eb="3">
+      <t>カンリョウビ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2020/11/28</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>見積
+(相対)</t>
+    <rPh sb="0" eb="2">
+      <t>ミツモリ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>ソウタイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>テスト
+実装</t>
+    <rPh sb="4" eb="6">
+      <t>ジッソウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>利用者は[開始日時][終了日時]から算出された所要時間を確認できる</t>
+    <rPh sb="0" eb="3">
+      <t>リヨウシャ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>サンシュツ</t>
+    </rPh>
+    <rPh sb="23" eb="27">
+      <t>ショヨウジカン</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>カクニン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>所要時間を知りたいから</t>
+    <rPh sb="0" eb="4">
+      <t>ショヨウジカン</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>シ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[開始日時][終了日時]の両方が入力されている場合、[保存]ボタンをクリックすると所要時間が表示される</t>
+    <rPh sb="13" eb="15">
+      <t>リョウホウ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="27" eb="29">
+      <t>ホゾン</t>
+    </rPh>
+    <rPh sb="41" eb="45">
+      <t>ショヨウジカン</t>
+    </rPh>
+    <rPh sb="46" eb="48">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>利用者は過去に入力した[開始日時][終了日時]と[所要時間]を確認できる</t>
+    <rPh sb="0" eb="3">
+      <t>リヨウシャ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>カコ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="25" eb="29">
+      <t>ショヨウジカン</t>
+    </rPh>
+    <rPh sb="31" eb="33">
+      <t>カクニン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>所要時間の変化を知りたいから</t>
+    <rPh sb="0" eb="4">
+      <t>ショヨウジカン</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ヘンカ</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>シ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>過去の[開始日時][終了日時]が入力されている場合、[表示]ボタンをクリックすると過去のデータが表示される</t>
+    <rPh sb="0" eb="2">
+      <t>カコ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="27" eb="29">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="41" eb="43">
+      <t>カコ</t>
+    </rPh>
+    <rPh sb="48" eb="50">
+      <t>ヒョウジ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -850,7 +978,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -860,6 +988,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -900,7 +1040,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -921,15 +1061,30 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -953,18 +1108,18 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>425450</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>196850</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3429144" cy="2389372"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="テキスト ボックス 1">
+        <xdr:cNvPr id="4" name="テキスト ボックス 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1BA99428-1597-42BF-8DF1-42522348767D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2124341B-71F0-4F28-87F4-E90ACE46D9DD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -972,7 +1127,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1085850" y="1111250"/>
+          <a:off x="511969" y="904875"/>
           <a:ext cx="3429144" cy="2389372"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1111,17 +1266,17 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>222250</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1736373" cy="1036694"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="テキスト ボックス 2">
+        <xdr:cNvPr id="6" name="テキスト ボックス 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CECFB488-D760-4457-8090-98AF90A5213F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D02A1F08-1D8A-4D8B-8F44-3D9280E1CAED}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1129,7 +1284,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5372100" y="1136650"/>
+          <a:off x="6560344" y="904875"/>
           <a:ext cx="1736373" cy="1036694"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1208,16 +1363,16 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>105938</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>149902</xdr:rowOff>
+      <xdr:colOff>125781</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>46714</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="図 1">
+        <xdr:cNvPr id="4" name="図 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A637BA2B-3A0E-4FFE-8ED1-558E40F6AB30}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA7E6FAA-DDAE-403E-A54D-A9B0B78AEE52}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1233,7 +1388,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="198438" y="1150938"/>
+          <a:off x="202406" y="1131094"/>
           <a:ext cx="3400000" cy="7285714"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1513,10 +1668,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:AA31"/>
+  <dimension ref="A2:AB34"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A14" zoomScale="80" zoomScaleNormal="60" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="T25" sqref="T25"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A25" zoomScale="80" zoomScaleNormal="60" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -1526,19 +1681,24 @@
     <col min="3" max="3" width="25.58203125" style="2" customWidth="1"/>
     <col min="4" max="4" width="28.08203125" style="2" customWidth="1" outlineLevel="1"/>
     <col min="5" max="5" width="25.58203125" style="2" customWidth="1"/>
-    <col min="6" max="8" width="8.6640625" style="1"/>
-    <col min="9" max="10" width="25.58203125" style="2" customWidth="1"/>
-    <col min="11" max="16" width="8.6640625" style="1"/>
-    <col min="17" max="19" width="8.6640625" style="3"/>
-    <col min="20" max="20" width="8.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="8.6640625" style="1"/>
+    <col min="6" max="6" width="8.6640625" style="1"/>
+    <col min="7" max="7" width="8.6640625" style="1" collapsed="1"/>
+    <col min="8" max="8" width="8.6640625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="12.58203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="25.58203125" style="2" customWidth="1"/>
+    <col min="12" max="16" width="8.6640625" style="1"/>
+    <col min="17" max="18" width="8.6640625" style="3"/>
+    <col min="19" max="19" width="8.6640625" style="3" collapsed="1"/>
+    <col min="20" max="20" width="0" style="3" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="21" max="21" width="8.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:2">
       <c r="B2" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="2:2">
@@ -1546,515 +1706,677 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:27" s="2" customFormat="1" ht="36" collapsed="1">
-      <c r="A18" s="10"/>
-      <c r="B18" s="7" t="s">
+    <row r="17" spans="1:28" s="2" customFormat="1" ht="36" collapsed="1">
+      <c r="A17" s="9"/>
+      <c r="B17" s="13" t="s">
         <v>3</v>
       </c>
+      <c r="C17" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="H17" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I17" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="J17" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="K17" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="L17" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="M17" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="N17" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="O17" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="P17" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q17" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="R17" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="S17" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="T17" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="U17" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="V17" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="W17" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="X17" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB17" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" hidden="1" outlineLevel="1">
+      <c r="B18" s="7"/>
       <c r="C18" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="6"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="7"/>
+      <c r="T18" s="7"/>
+      <c r="U18" s="7"/>
+      <c r="V18" s="8"/>
+      <c r="W18" s="8"/>
+      <c r="X18" s="8"/>
+    </row>
+    <row r="19" spans="1:28" ht="54">
+      <c r="B19" s="10">
+        <v>1</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" s="11"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="J19" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="K19" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="L19" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="12"/>
+      <c r="Q19" s="10">
+        <v>1</v>
+      </c>
+      <c r="R19" s="10">
+        <v>1</v>
+      </c>
+      <c r="S19" s="10"/>
+      <c r="T19" s="10"/>
+      <c r="U19" s="10">
+        <v>1</v>
+      </c>
+      <c r="V19" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="W19" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="X19" s="12"/>
+    </row>
+    <row r="20" spans="1:28" ht="36">
+      <c r="B20" s="10"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="12"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="10"/>
+      <c r="T20" s="10"/>
+      <c r="U20" s="10"/>
+      <c r="V20" s="12"/>
+      <c r="W20" s="12"/>
+      <c r="X20" s="12"/>
+    </row>
+    <row r="21" spans="1:28" ht="36">
+      <c r="B21" s="10"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
+      <c r="P21" s="12"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="10"/>
+      <c r="S21" s="10"/>
+      <c r="T21" s="10"/>
+      <c r="U21" s="10"/>
+      <c r="V21" s="12"/>
+      <c r="W21" s="12"/>
+      <c r="X21" s="12"/>
+    </row>
+    <row r="22" spans="1:28" ht="36">
+      <c r="B22" s="10"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
+      <c r="P22" s="12"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="10"/>
+      <c r="S22" s="10"/>
+      <c r="T22" s="10"/>
+      <c r="U22" s="10"/>
+      <c r="V22" s="12"/>
+      <c r="W22" s="12"/>
+      <c r="X22" s="12"/>
+    </row>
+    <row r="23" spans="1:28" ht="36">
+      <c r="B23" s="10"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="M23" s="12"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="12"/>
+      <c r="P23" s="12"/>
+      <c r="Q23" s="10"/>
+      <c r="R23" s="10"/>
+      <c r="S23" s="10"/>
+      <c r="T23" s="10"/>
+      <c r="U23" s="10"/>
+      <c r="V23" s="12"/>
+      <c r="W23" s="12"/>
+      <c r="X23" s="12"/>
+    </row>
+    <row r="24" spans="1:28" ht="36">
+      <c r="B24" s="10">
+        <v>2</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E24" s="11"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="L24" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="M24" s="12"/>
+      <c r="N24" s="12"/>
+      <c r="O24" s="12"/>
+      <c r="P24" s="12"/>
+      <c r="Q24" s="10">
+        <v>3</v>
+      </c>
+      <c r="R24" s="10">
+        <f>SUM(S25:S26)</f>
+        <v>3</v>
+      </c>
+      <c r="S24" s="10"/>
+      <c r="T24" s="10"/>
+      <c r="U24" s="10"/>
+      <c r="V24" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="W24" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="X24" s="12"/>
+    </row>
+    <row r="25" spans="1:28" ht="36">
+      <c r="B25" s="10"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="M25" s="12"/>
+      <c r="N25" s="12"/>
+      <c r="O25" s="12"/>
+      <c r="P25" s="12"/>
+      <c r="Q25" s="10"/>
+      <c r="R25" s="10"/>
+      <c r="S25" s="10">
+        <v>1</v>
+      </c>
+      <c r="T25" s="10"/>
+      <c r="U25" s="10">
+        <v>1</v>
+      </c>
+      <c r="V25" s="12"/>
+      <c r="W25" s="12"/>
+      <c r="X25" s="12"/>
+    </row>
+    <row r="26" spans="1:28" ht="54">
+      <c r="B26" s="10"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="K26" s="11"/>
+      <c r="L26" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="M26" s="12"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="12"/>
+      <c r="P26" s="12"/>
+      <c r="Q26" s="10"/>
+      <c r="R26" s="10"/>
+      <c r="S26" s="10">
+        <v>2</v>
+      </c>
+      <c r="T26" s="10"/>
+      <c r="U26" s="10">
+        <v>1</v>
+      </c>
+      <c r="V26" s="12"/>
+      <c r="W26" s="12"/>
+      <c r="X26" s="12"/>
+    </row>
+    <row r="27" spans="1:28" ht="72">
+      <c r="B27" s="10">
+        <v>3</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E27" s="11"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="12"/>
+      <c r="P27" s="12"/>
+      <c r="Q27" s="10"/>
+      <c r="R27" s="10"/>
+      <c r="S27" s="10">
+        <v>1</v>
+      </c>
+      <c r="T27" s="10"/>
+      <c r="U27" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="V27" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="W27" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="X27" s="12"/>
+    </row>
+    <row r="28" spans="1:28" ht="54">
+      <c r="B28" s="10"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="M28" s="12"/>
+      <c r="N28" s="12"/>
+      <c r="O28" s="12"/>
+      <c r="P28" s="12"/>
+      <c r="Q28" s="10"/>
+      <c r="R28" s="10"/>
+      <c r="S28" s="10"/>
+      <c r="T28" s="10"/>
+      <c r="U28" s="10"/>
+      <c r="V28" s="12"/>
+      <c r="W28" s="12"/>
+      <c r="X28" s="12"/>
+    </row>
+    <row r="29" spans="1:28" ht="54">
+      <c r="B29" s="7">
+        <v>5</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E29" s="6"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="M29" s="8"/>
+      <c r="N29" s="8"/>
+      <c r="O29" s="8"/>
+      <c r="P29" s="8"/>
+      <c r="Q29" s="7"/>
+      <c r="R29" s="7"/>
+      <c r="S29" s="7"/>
+      <c r="T29" s="7"/>
+      <c r="U29" s="7"/>
+      <c r="V29" s="8"/>
+      <c r="W29" s="8"/>
+      <c r="X29" s="8"/>
+    </row>
+    <row r="30" spans="1:28" ht="72">
+      <c r="B30" s="7"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="M30" s="8"/>
+      <c r="N30" s="8"/>
+      <c r="O30" s="8"/>
+      <c r="P30" s="8"/>
+      <c r="Q30" s="7"/>
+      <c r="R30" s="7"/>
+      <c r="S30" s="7"/>
+      <c r="T30" s="7"/>
+      <c r="U30" s="7"/>
+      <c r="V30" s="8"/>
+      <c r="W30" s="8"/>
+      <c r="X30" s="8"/>
+    </row>
+    <row r="31" spans="1:28" ht="54">
+      <c r="B31" s="7">
+        <v>6</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E31" s="6"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="M31" s="8"/>
+      <c r="N31" s="8"/>
+      <c r="O31" s="8"/>
+      <c r="P31" s="8"/>
+      <c r="Q31" s="7"/>
+      <c r="R31" s="7"/>
+      <c r="S31" s="7"/>
+      <c r="T31" s="7"/>
+      <c r="U31" s="7"/>
+      <c r="V31" s="8"/>
+      <c r="W31" s="8"/>
+      <c r="X31" s="8"/>
+    </row>
+    <row r="32" spans="1:28" ht="72">
+      <c r="B32" s="7"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="M32" s="8"/>
+      <c r="N32" s="8"/>
+      <c r="O32" s="8"/>
+      <c r="P32" s="8"/>
+      <c r="Q32" s="7"/>
+      <c r="R32" s="7"/>
+      <c r="S32" s="7"/>
+      <c r="T32" s="7"/>
+      <c r="U32" s="7"/>
+      <c r="V32" s="8"/>
+      <c r="W32" s="8"/>
+      <c r="X32" s="8"/>
+    </row>
+    <row r="33" spans="2:24" ht="54">
+      <c r="B33" s="7">
         <v>4</v>
       </c>
-      <c r="F18" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I18" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="J18" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="K18" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="L18" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="M18" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="N18" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="O18" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="P18" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q18" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="R18" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="S18" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="T18" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="U18" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="V18" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="W18" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="X18" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y18" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="Z18" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AA18" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:27" hidden="1" outlineLevel="1">
-      <c r="B19" s="8"/>
-      <c r="C19" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E19" s="6"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="9"/>
-      <c r="O19" s="9"/>
-      <c r="P19" s="9"/>
-      <c r="Q19" s="8"/>
-      <c r="R19" s="8"/>
-      <c r="S19" s="8"/>
-      <c r="T19" s="8"/>
-      <c r="U19" s="9"/>
-      <c r="V19" s="9"/>
-      <c r="W19" s="9"/>
-    </row>
-    <row r="20" spans="1:27" ht="54">
-      <c r="B20" s="8">
-        <v>1</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E20" s="6"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="J20" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="K20" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="9"/>
-      <c r="Q20" s="8">
-        <v>1</v>
-      </c>
-      <c r="R20" s="8"/>
-      <c r="S20" s="8"/>
-      <c r="T20" s="8">
-        <v>1</v>
-      </c>
-      <c r="U20" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="V20" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="W20" s="9"/>
-    </row>
-    <row r="21" spans="1:27" ht="36">
-      <c r="B21" s="8"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="H21" s="9"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9"/>
-      <c r="N21" s="9"/>
-      <c r="O21" s="9"/>
-      <c r="P21" s="9"/>
-      <c r="Q21" s="8"/>
-      <c r="R21" s="8"/>
-      <c r="S21" s="8"/>
-      <c r="T21" s="8"/>
-      <c r="U21" s="9"/>
-      <c r="V21" s="9"/>
-      <c r="W21" s="9"/>
-    </row>
-    <row r="22" spans="1:27" ht="36">
-      <c r="B22" s="8"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6" t="s">
+      <c r="C33" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E33" s="6"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="M33" s="8"/>
+      <c r="N33" s="8"/>
+      <c r="O33" s="8"/>
+      <c r="P33" s="8"/>
+      <c r="Q33" s="7"/>
+      <c r="R33" s="7"/>
+      <c r="S33" s="7"/>
+      <c r="T33" s="7"/>
+      <c r="U33" s="7"/>
+      <c r="V33" s="8"/>
+      <c r="W33" s="8"/>
+      <c r="X33" s="8"/>
+    </row>
+    <row r="34" spans="2:24" ht="54">
+      <c r="B34" s="7"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="H22" s="9"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="L22" s="9"/>
-      <c r="M22" s="9"/>
-      <c r="N22" s="9"/>
-      <c r="O22" s="9"/>
-      <c r="P22" s="9"/>
-      <c r="Q22" s="8"/>
-      <c r="R22" s="8"/>
-      <c r="S22" s="8"/>
-      <c r="T22" s="8"/>
-      <c r="U22" s="9"/>
-      <c r="V22" s="9"/>
-      <c r="W22" s="9"/>
-    </row>
-    <row r="23" spans="1:27" ht="36">
-      <c r="B23" s="8"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="H23" s="9"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="L23" s="9"/>
-      <c r="M23" s="9"/>
-      <c r="N23" s="9"/>
-      <c r="O23" s="9"/>
-      <c r="P23" s="9"/>
-      <c r="Q23" s="8"/>
-      <c r="R23" s="8"/>
-      <c r="S23" s="8"/>
-      <c r="T23" s="8"/>
-      <c r="U23" s="9"/>
-      <c r="V23" s="9"/>
-      <c r="W23" s="9"/>
-    </row>
-    <row r="24" spans="1:27" ht="36">
-      <c r="B24" s="8"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H24" s="9"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="L24" s="9"/>
-      <c r="M24" s="9"/>
-      <c r="N24" s="9"/>
-      <c r="O24" s="9"/>
-      <c r="P24" s="9"/>
-      <c r="Q24" s="8"/>
-      <c r="R24" s="8"/>
-      <c r="S24" s="8"/>
-      <c r="T24" s="8"/>
-      <c r="U24" s="9"/>
-      <c r="V24" s="9"/>
-      <c r="W24" s="9"/>
-    </row>
-    <row r="25" spans="1:27" ht="36">
-      <c r="B25" s="8">
-        <v>2</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E25" s="6"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="K25" s="9"/>
-      <c r="L25" s="9"/>
-      <c r="M25" s="9"/>
-      <c r="N25" s="9"/>
-      <c r="O25" s="9"/>
-      <c r="P25" s="9"/>
-      <c r="Q25" s="8">
-        <f>SUM(R26:R27)</f>
-        <v>3</v>
-      </c>
-      <c r="R25" s="8"/>
-      <c r="S25" s="8"/>
-      <c r="T25" s="8"/>
-      <c r="U25" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="V25" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="W25" s="9"/>
-    </row>
-    <row r="26" spans="1:27" ht="36">
-      <c r="B26" s="8"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="H26" s="9"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="L26" s="9"/>
-      <c r="M26" s="9"/>
-      <c r="N26" s="9"/>
-      <c r="O26" s="9"/>
-      <c r="P26" s="9"/>
-      <c r="Q26" s="8"/>
-      <c r="R26" s="8">
-        <v>1</v>
-      </c>
-      <c r="S26" s="8"/>
-      <c r="T26" s="8">
-        <v>1</v>
-      </c>
-      <c r="U26" s="9"/>
-      <c r="V26" s="9"/>
-      <c r="W26" s="9"/>
-    </row>
-    <row r="27" spans="1:27" ht="54">
-      <c r="B27" s="8"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="H27" s="9"/>
-      <c r="I27" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="J27" s="6"/>
-      <c r="K27" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="L27" s="9"/>
-      <c r="M27" s="9"/>
-      <c r="N27" s="9"/>
-      <c r="O27" s="9"/>
-      <c r="P27" s="9"/>
-      <c r="Q27" s="8"/>
-      <c r="R27" s="8">
-        <v>2</v>
-      </c>
-      <c r="S27" s="8"/>
-      <c r="T27" s="8"/>
-      <c r="U27" s="9"/>
-      <c r="V27" s="9"/>
-      <c r="W27" s="9"/>
-    </row>
-    <row r="28" spans="1:27" ht="72">
-      <c r="B28" s="8">
-        <v>3</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="9"/>
-      <c r="L28" s="9"/>
-      <c r="M28" s="9"/>
-      <c r="N28" s="9"/>
-      <c r="O28" s="9"/>
-      <c r="P28" s="9"/>
-      <c r="Q28" s="8"/>
-      <c r="R28" s="8"/>
-      <c r="S28" s="8"/>
-      <c r="T28" s="8"/>
-      <c r="U28" s="9"/>
-      <c r="V28" s="9"/>
-      <c r="W28" s="9"/>
-    </row>
-    <row r="29" spans="1:27" ht="54">
-      <c r="B29" s="8"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
-      <c r="K29" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="L29" s="9"/>
-      <c r="M29" s="9"/>
-      <c r="N29" s="9"/>
-      <c r="O29" s="9"/>
-      <c r="P29" s="9"/>
-      <c r="Q29" s="8"/>
-      <c r="R29" s="8"/>
-      <c r="S29" s="8"/>
-      <c r="T29" s="8"/>
-      <c r="U29" s="9"/>
-      <c r="V29" s="9"/>
-      <c r="W29" s="9"/>
-    </row>
-    <row r="30" spans="1:27" ht="54">
-      <c r="B30" s="8">
-        <v>4</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="6"/>
-      <c r="K30" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="L30" s="9"/>
-      <c r="M30" s="9"/>
-      <c r="N30" s="9"/>
-      <c r="O30" s="9"/>
-      <c r="P30" s="9"/>
-      <c r="Q30" s="8"/>
-      <c r="R30" s="8"/>
-      <c r="S30" s="8"/>
-      <c r="T30" s="8"/>
-      <c r="U30" s="9"/>
-      <c r="V30" s="9"/>
-      <c r="W30" s="9"/>
-    </row>
-    <row r="31" spans="1:27" ht="54">
-      <c r="B31" s="8"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
-      <c r="K31" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="L31" s="9"/>
-      <c r="M31" s="9"/>
-      <c r="N31" s="9"/>
-      <c r="O31" s="9"/>
-      <c r="P31" s="9"/>
-      <c r="Q31" s="8"/>
-      <c r="R31" s="8"/>
-      <c r="S31" s="8"/>
-      <c r="T31" s="8"/>
-      <c r="U31" s="9"/>
-      <c r="V31" s="9"/>
-      <c r="W31" s="9"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="6"/>
+      <c r="L34" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="M34" s="8"/>
+      <c r="N34" s="8"/>
+      <c r="O34" s="8"/>
+      <c r="P34" s="8"/>
+      <c r="Q34" s="7"/>
+      <c r="R34" s="7"/>
+      <c r="S34" s="7"/>
+      <c r="T34" s="7"/>
+      <c r="U34" s="7"/>
+      <c r="V34" s="8"/>
+      <c r="W34" s="8"/>
+      <c r="X34" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K20:K31" xr:uid="{28DE5D51-C321-4870-B1C8-48B479072D32}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L19:L34" xr:uid="{28DE5D51-C321-4870-B1C8-48B479072D32}">
       <formula1>"タスク,税,Spike,前提条件(技術的負債)"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="43" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="41" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;F　&amp;A&amp;R&amp;D　&amp;T</oddHeader>
     <oddFooter>&amp;C&amp;P</oddFooter>
@@ -2080,17 +2402,17 @@
   <sheetData>
     <row r="2" spans="2:4">
       <c r="B2" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="2:4">
       <c r="B3" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="2:4">
       <c r="B4" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="2:4">
@@ -2098,7 +2420,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D6" s="5"/>
     </row>
@@ -2107,7 +2429,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D7" s="5"/>
     </row>
@@ -2116,7 +2438,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D8" s="5"/>
     </row>
@@ -2125,7 +2447,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D9" s="5"/>
     </row>
@@ -2134,88 +2456,88 @@
         <v>5</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D10" s="5"/>
     </row>
     <row r="11" spans="2:4">
       <c r="C11" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="2:4">
       <c r="C12" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="2:4">
       <c r="C13" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="2:4">
       <c r="C14" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="2:4">
       <c r="C15" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="2:4">
       <c r="C16" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="2:4">
       <c r="C17" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="2:4">
       <c r="C18" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="2:4">
       <c r="C19" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="2:4">
       <c r="C20" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="2:4">
@@ -2223,7 +2545,7 @@
         <v>6</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D21" s="5"/>
     </row>
@@ -2232,7 +2554,7 @@
         <v>7</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D22" s="5"/>
     </row>
@@ -2241,23 +2563,23 @@
         <v>10</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="2:4">
       <c r="C25" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="2:4">
       <c r="C26" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="2:4">
@@ -2265,23 +2587,23 @@
         <v>11</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="2:4">
       <c r="C28" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="2:4">
       <c r="C29" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="2:4">
@@ -2289,23 +2611,23 @@
         <v>12</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="2:4">
       <c r="C31" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32" spans="2:4">
       <c r="C32" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2326,8 +2648,8 @@
   </sheetPr>
   <dimension ref="B2:L18"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -2350,36 +2672,36 @@
     </row>
     <row r="12" spans="2:12">
       <c r="I12" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="2:12">
       <c r="I14" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L14" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="15" spans="2:12">
       <c r="I15" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="2:12">
       <c r="I16" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="9:10">
       <c r="I18" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* Add function to show db contents.
</commit_message>
<xml_diff>
--- a/doc/TimeSavingBox.xlsx
+++ b/doc/TimeSavingBox.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\develop\work\AndroidStudioProjects\TimeSavingBox\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D6A66B-249A-4295-95F8-4EF8BA0E987A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E3CC242-568F-4FCC-8E35-2EED0F84FA8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36300" yWindow="690" windowWidth="23040" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="285" yWindow="2325" windowWidth="21600" windowHeight="12915" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="プロダクトバックログ" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="dummy" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">プロダクトバックログ!$A$1:$X$34</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">プロダクトバックログ!$A$1:$G$51</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="124">
   <si>
     <t>■dummy</t>
     <phoneticPr fontId="1"/>
@@ -938,6 +938,34 @@
     <rPh sb="48" eb="50">
       <t>ヒョウジ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;2&gt;2020-12-31</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>timesavingbox.db</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>_id</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>date</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>starttime</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>endtime</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>memo</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -978,7 +1006,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1000,6 +1028,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1040,7 +1074,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1087,12 +1121,20 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFCCFF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1110,7 +1152,7 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3429144" cy="2389372"/>
@@ -1267,7 +1309,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1736373" cy="1036694"/>
@@ -1356,15 +1398,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>125781</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>46714</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1396,6 +1438,154 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>35718</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>416718</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>214312</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="吹き出し: 角を丸めた四角形 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{935E920C-915C-4E01-96E9-6AADA26D14FF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4822031" y="1428750"/>
+          <a:ext cx="2524125" cy="1166812"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -103153"/>
+            <a:gd name="adj2" fmla="val 140051"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFCCFF"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>時間の計算結果を表示してほしい</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>35718</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>59532</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>416718</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>35719</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="吹き出し: 角を丸めた四角形 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CFF3A69-57B4-4AC2-A942-5D1EE1A6299D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4822031" y="5060157"/>
+          <a:ext cx="2524125" cy="1166812"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -93719"/>
+            <a:gd name="adj2" fmla="val -68112"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFCCFF"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>過去時間を取得したい</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1668,32 +1858,32 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:AB34"/>
+  <dimension ref="A2:AB35"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A25" zoomScale="80" zoomScaleNormal="60" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A30" zoomScale="80" zoomScaleNormal="60" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="18.75" outlineLevelRow="1" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="2.58203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="4.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.58203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="28.08203125" style="2" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="25.58203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="8.6640625" style="1"/>
-    <col min="7" max="7" width="8.6640625" style="1" collapsed="1"/>
-    <col min="8" max="8" width="8.6640625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="12.58203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="25.58203125" style="2" customWidth="1"/>
-    <col min="12" max="16" width="8.6640625" style="1"/>
-    <col min="17" max="18" width="8.6640625" style="3"/>
-    <col min="19" max="19" width="8.6640625" style="3" collapsed="1"/>
+    <col min="1" max="1" width="2.625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="4.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="28.125" style="2" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="25.625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="8.625" style="1"/>
+    <col min="7" max="7" width="8.625" style="1" collapsed="1"/>
+    <col min="8" max="8" width="8.625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="12.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="25.625" style="2" customWidth="1"/>
+    <col min="12" max="16" width="8.625" style="1"/>
+    <col min="17" max="18" width="8.625" style="3"/>
+    <col min="19" max="19" width="8.625" style="3" collapsed="1"/>
     <col min="20" max="20" width="0" style="3" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="21" max="21" width="8.5" style="3" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="12.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="8.6640625" style="1"/>
+    <col min="23" max="23" width="8.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="8.625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:2">
@@ -1706,185 +1896,149 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:28" s="2" customFormat="1" ht="36" collapsed="1">
-      <c r="A17" s="9"/>
-      <c r="B17" s="13" t="s">
+    <row r="4" spans="2:2">
+      <c r="B4" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" s="2" customFormat="1" ht="37.5" collapsed="1">
+      <c r="A18" s="9"/>
+      <c r="B18" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C18" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D18" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E18" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F17" s="14" t="s">
+      <c r="F18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G17" s="14" t="s">
+      <c r="G18" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="H17" s="14" t="s">
+      <c r="H18" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="I17" s="14" t="s">
+      <c r="I18" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="J17" s="14" t="s">
+      <c r="J18" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="K17" s="14" t="s">
+      <c r="K18" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="L17" s="14" t="s">
+      <c r="L18" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="M17" s="14" t="s">
+      <c r="M18" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="N17" s="14" t="s">
+      <c r="N18" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="O17" s="14" t="s">
+      <c r="O18" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="P17" s="14" t="s">
+      <c r="P18" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="Q17" s="13" t="s">
+      <c r="Q18" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="R17" s="13" t="s">
+      <c r="R18" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="S17" s="13" t="s">
+      <c r="S18" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="T17" s="13" t="s">
+      <c r="T18" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="U17" s="13" t="s">
+      <c r="U18" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="V17" s="14" t="s">
+      <c r="V18" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="W17" s="14" t="s">
+      <c r="W18" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="X17" s="14" t="s">
+      <c r="X18" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="Y17" s="2" t="s">
+      <c r="Y18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="Z17" s="2" t="s">
+      <c r="Z18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="AA17" s="2" t="s">
+      <c r="AA18" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="AB17" s="2" t="s">
+      <c r="AB18" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:28" hidden="1" outlineLevel="1">
-      <c r="B18" s="7"/>
-      <c r="C18" s="6" t="s">
+    <row r="19" spans="1:28" hidden="1" outlineLevel="1">
+      <c r="B19" s="7"/>
+      <c r="C19" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D19" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="6"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6" t="s">
+      <c r="E19" s="6"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8"/>
-      <c r="P18" s="8"/>
-      <c r="Q18" s="7"/>
-      <c r="R18" s="7"/>
-      <c r="S18" s="7"/>
-      <c r="T18" s="7"/>
-      <c r="U18" s="7"/>
-      <c r="V18" s="8"/>
-      <c r="W18" s="8"/>
-      <c r="X18" s="8"/>
-    </row>
-    <row r="19" spans="1:28" ht="54">
-      <c r="B19" s="10">
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
+      <c r="U19" s="7"/>
+      <c r="V19" s="8"/>
+      <c r="W19" s="8"/>
+      <c r="X19" s="8"/>
+    </row>
+    <row r="20" spans="1:28" ht="75">
+      <c r="B20" s="10">
         <v>1</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C20" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D20" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="E19" s="11"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12" t="s">
+      <c r="E20" s="11"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="J19" s="11" t="s">
+      <c r="J20" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="K19" s="11" t="s">
+      <c r="K20" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="L19" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="M19" s="12"/>
-      <c r="N19" s="12"/>
-      <c r="O19" s="12"/>
-      <c r="P19" s="12"/>
-      <c r="Q19" s="10">
-        <v>1</v>
-      </c>
-      <c r="R19" s="10">
-        <v>1</v>
-      </c>
-      <c r="S19" s="10"/>
-      <c r="T19" s="10"/>
-      <c r="U19" s="10">
-        <v>1</v>
-      </c>
-      <c r="V19" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="W19" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="X19" s="12"/>
-    </row>
-    <row r="20" spans="1:28" ht="36">
-      <c r="B20" s="10"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="11"/>
       <c r="L20" s="12" t="s">
         <v>98</v>
       </c>
@@ -1892,25 +2046,35 @@
       <c r="N20" s="12"/>
       <c r="O20" s="12"/>
       <c r="P20" s="12"/>
-      <c r="Q20" s="10"/>
-      <c r="R20" s="10"/>
+      <c r="Q20" s="10">
+        <v>1</v>
+      </c>
+      <c r="R20" s="10">
+        <v>1</v>
+      </c>
       <c r="S20" s="10"/>
       <c r="T20" s="10"/>
-      <c r="U20" s="10"/>
-      <c r="V20" s="12"/>
-      <c r="W20" s="12"/>
+      <c r="U20" s="10">
+        <v>1</v>
+      </c>
+      <c r="V20" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="W20" s="12" t="s">
+        <v>99</v>
+      </c>
       <c r="X20" s="12"/>
     </row>
-    <row r="21" spans="1:28" ht="36">
+    <row r="21" spans="1:28" ht="37.5">
       <c r="B21" s="10"/>
       <c r="C21" s="11"/>
       <c r="D21" s="11"/>
       <c r="E21" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F21" s="12"/>
       <c r="G21" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H21" s="12"/>
       <c r="I21" s="12"/>
@@ -1932,16 +2096,16 @@
       <c r="W21" s="12"/>
       <c r="X21" s="12"/>
     </row>
-    <row r="22" spans="1:28" ht="36">
+    <row r="22" spans="1:28" ht="37.5">
       <c r="B22" s="10"/>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
       <c r="E22" s="11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F22" s="12"/>
       <c r="G22" s="12" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="H22" s="12"/>
       <c r="I22" s="12"/>
@@ -1963,16 +2127,16 @@
       <c r="W22" s="12"/>
       <c r="X22" s="12"/>
     </row>
-    <row r="23" spans="1:28" ht="36">
+    <row r="23" spans="1:28" ht="37.5">
       <c r="B23" s="10"/>
       <c r="C23" s="11"/>
       <c r="D23" s="11"/>
       <c r="E23" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F23" s="12"/>
       <c r="G23" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H23" s="12"/>
       <c r="I23" s="12"/>
@@ -1994,27 +2158,21 @@
       <c r="W23" s="12"/>
       <c r="X23" s="12"/>
     </row>
-    <row r="24" spans="1:28" ht="36">
-      <c r="B24" s="10">
-        <v>2</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="E24" s="11"/>
+    <row r="24" spans="1:28" ht="37.5">
+      <c r="B24" s="10"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11" t="s">
+        <v>35</v>
+      </c>
       <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
+      <c r="G24" s="12" t="s">
+        <v>30</v>
+      </c>
       <c r="H24" s="12"/>
-      <c r="I24" s="12" t="s">
-        <v>108</v>
-      </c>
+      <c r="I24" s="12"/>
       <c r="J24" s="11"/>
-      <c r="K24" s="11" t="s">
-        <v>103</v>
-      </c>
+      <c r="K24" s="11"/>
       <c r="L24" s="12" t="s">
         <v>98</v>
       </c>
@@ -2022,39 +2180,36 @@
       <c r="N24" s="12"/>
       <c r="O24" s="12"/>
       <c r="P24" s="12"/>
-      <c r="Q24" s="10">
-        <v>3</v>
-      </c>
-      <c r="R24" s="10">
-        <f>SUM(S25:S26)</f>
-        <v>3</v>
-      </c>
+      <c r="Q24" s="10"/>
+      <c r="R24" s="10"/>
       <c r="S24" s="10"/>
       <c r="T24" s="10"/>
       <c r="U24" s="10"/>
-      <c r="V24" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="W24" s="12" t="s">
-        <v>99</v>
-      </c>
+      <c r="V24" s="12"/>
+      <c r="W24" s="12"/>
       <c r="X24" s="12"/>
     </row>
-    <row r="25" spans="1:28" ht="36">
-      <c r="B25" s="10"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11" t="s">
-        <v>36</v>
-      </c>
+    <row r="25" spans="1:28" ht="37.5">
+      <c r="B25" s="10">
+        <v>2</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" s="11"/>
       <c r="F25" s="12"/>
-      <c r="G25" s="12" t="s">
-        <v>33</v>
-      </c>
+      <c r="G25" s="12"/>
       <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
+      <c r="I25" s="12" t="s">
+        <v>108</v>
+      </c>
       <c r="J25" s="11"/>
-      <c r="K25" s="11"/>
+      <c r="K25" s="11" t="s">
+        <v>103</v>
+      </c>
       <c r="L25" s="12" t="s">
         <v>98</v>
       </c>
@@ -2062,35 +2217,38 @@
       <c r="N25" s="12"/>
       <c r="O25" s="12"/>
       <c r="P25" s="12"/>
-      <c r="Q25" s="10"/>
-      <c r="R25" s="10"/>
-      <c r="S25" s="10">
-        <v>1</v>
-      </c>
+      <c r="Q25" s="10">
+        <v>3</v>
+      </c>
+      <c r="R25" s="10">
+        <f>SUM(S26:S27)</f>
+        <v>3</v>
+      </c>
+      <c r="S25" s="10"/>
       <c r="T25" s="10"/>
-      <c r="U25" s="10">
-        <v>1</v>
-      </c>
-      <c r="V25" s="12"/>
-      <c r="W25" s="12"/>
+      <c r="U25" s="10"/>
+      <c r="V25" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="W25" s="12" t="s">
+        <v>99</v>
+      </c>
       <c r="X25" s="12"/>
     </row>
-    <row r="26" spans="1:28" ht="54">
+    <row r="26" spans="1:28" ht="37.5">
       <c r="B26" s="10"/>
       <c r="C26" s="11"/>
       <c r="D26" s="11"/>
       <c r="E26" s="11" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="F26" s="12"/>
       <c r="G26" s="12" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="H26" s="12"/>
       <c r="I26" s="12"/>
-      <c r="J26" s="11" t="s">
-        <v>101</v>
-      </c>
+      <c r="J26" s="11"/>
       <c r="K26" s="11"/>
       <c r="L26" s="12" t="s">
         <v>98</v>
@@ -2102,7 +2260,7 @@
       <c r="Q26" s="10"/>
       <c r="R26" s="10"/>
       <c r="S26" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T26" s="10"/>
       <c r="U26" s="10">
@@ -2112,22 +2270,22 @@
       <c r="W26" s="12"/>
       <c r="X26" s="12"/>
     </row>
-    <row r="27" spans="1:28" ht="72">
-      <c r="B27" s="10">
-        <v>3</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="E27" s="11"/>
+    <row r="27" spans="1:28" ht="56.25">
+      <c r="B27" s="10"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11" t="s">
+        <v>102</v>
+      </c>
       <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
+      <c r="G27" s="12" t="s">
+        <v>45</v>
+      </c>
       <c r="H27" s="12"/>
       <c r="I27" s="12"/>
-      <c r="J27" s="11"/>
+      <c r="J27" s="11" t="s">
+        <v>101</v>
+      </c>
       <c r="K27" s="11"/>
       <c r="L27" s="12" t="s">
         <v>98</v>
@@ -2139,27 +2297,27 @@
       <c r="Q27" s="10"/>
       <c r="R27" s="10"/>
       <c r="S27" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T27" s="10"/>
       <c r="U27" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="V27" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="W27" s="12" t="s">
-        <v>99</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="V27" s="12"/>
+      <c r="W27" s="12"/>
       <c r="X27" s="12"/>
     </row>
-    <row r="28" spans="1:28" ht="54">
-      <c r="B28" s="10"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11" t="s">
-        <v>40</v>
-      </c>
+    <row r="28" spans="1:28" ht="75">
+      <c r="B28" s="10">
+        <v>3</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E28" s="11"/>
       <c r="F28" s="12"/>
       <c r="G28" s="12"/>
       <c r="H28" s="12"/>
@@ -2175,53 +2333,61 @@
       <c r="P28" s="12"/>
       <c r="Q28" s="10"/>
       <c r="R28" s="10"/>
-      <c r="S28" s="10"/>
+      <c r="S28" s="10">
+        <v>1</v>
+      </c>
       <c r="T28" s="10"/>
-      <c r="U28" s="10"/>
-      <c r="V28" s="12"/>
-      <c r="W28" s="12"/>
+      <c r="U28" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="V28" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="W28" s="12" t="s">
+        <v>99</v>
+      </c>
       <c r="X28" s="12"/>
     </row>
-    <row r="29" spans="1:28" ht="54">
-      <c r="B29" s="7">
+    <row r="29" spans="1:28" ht="56.25">
+      <c r="B29" s="10"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="M29" s="12"/>
+      <c r="N29" s="12"/>
+      <c r="O29" s="12"/>
+      <c r="P29" s="12"/>
+      <c r="Q29" s="10"/>
+      <c r="R29" s="10"/>
+      <c r="S29" s="10"/>
+      <c r="T29" s="10"/>
+      <c r="U29" s="10"/>
+      <c r="V29" s="12"/>
+      <c r="W29" s="12"/>
+      <c r="X29" s="12"/>
+    </row>
+    <row r="30" spans="1:28" ht="56.25">
+      <c r="B30" s="7">
         <v>5</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C30" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="D30" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="E29" s="6"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="6"/>
-      <c r="K29" s="6"/>
-      <c r="L29" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="M29" s="8"/>
-      <c r="N29" s="8"/>
-      <c r="O29" s="8"/>
-      <c r="P29" s="8"/>
-      <c r="Q29" s="7"/>
-      <c r="R29" s="7"/>
-      <c r="S29" s="7"/>
-      <c r="T29" s="7"/>
-      <c r="U29" s="7"/>
-      <c r="V29" s="8"/>
-      <c r="W29" s="8"/>
-      <c r="X29" s="8"/>
-    </row>
-    <row r="30" spans="1:28" ht="72">
-      <c r="B30" s="7"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="15" t="s">
-        <v>113</v>
-      </c>
+      <c r="E30" s="6"/>
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
@@ -2244,17 +2410,13 @@
       <c r="W30" s="8"/>
       <c r="X30" s="8"/>
     </row>
-    <row r="31" spans="1:28" ht="54">
-      <c r="B31" s="7">
-        <v>6</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="E31" s="6"/>
+    <row r="31" spans="1:28" ht="75">
+      <c r="B31" s="7"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="15" t="s">
+        <v>113</v>
+      </c>
       <c r="F31" s="8"/>
       <c r="G31" s="8"/>
       <c r="H31" s="8"/>
@@ -2277,13 +2439,17 @@
       <c r="W31" s="8"/>
       <c r="X31" s="8"/>
     </row>
-    <row r="32" spans="1:28" ht="72">
-      <c r="B32" s="7"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="15" t="s">
-        <v>116</v>
-      </c>
+    <row r="32" spans="1:28" ht="56.25">
+      <c r="B32" s="7">
+        <v>6</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E32" s="6"/>
       <c r="F32" s="8"/>
       <c r="G32" s="8"/>
       <c r="H32" s="8"/>
@@ -2306,17 +2472,13 @@
       <c r="W32" s="8"/>
       <c r="X32" s="8"/>
     </row>
-    <row r="33" spans="2:24" ht="54">
-      <c r="B33" s="7">
-        <v>4</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="E33" s="6"/>
+    <row r="33" spans="2:24" ht="75">
+      <c r="B33" s="7"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="15" t="s">
+        <v>116</v>
+      </c>
       <c r="F33" s="8"/>
       <c r="G33" s="8"/>
       <c r="H33" s="8"/>
@@ -2339,13 +2501,17 @@
       <c r="W33" s="8"/>
       <c r="X33" s="8"/>
     </row>
-    <row r="34" spans="2:24" ht="54">
-      <c r="B34" s="7"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6" t="s">
-        <v>39</v>
-      </c>
+    <row r="34" spans="2:24" ht="56.25">
+      <c r="B34" s="7">
+        <v>4</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E34" s="6"/>
       <c r="F34" s="8"/>
       <c r="G34" s="8"/>
       <c r="H34" s="8"/>
@@ -2368,19 +2534,51 @@
       <c r="W34" s="8"/>
       <c r="X34" s="8"/>
     </row>
+    <row r="35" spans="2:24" ht="56.25">
+      <c r="B35" s="7"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="6"/>
+      <c r="K35" s="6"/>
+      <c r="L35" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="M35" s="8"/>
+      <c r="N35" s="8"/>
+      <c r="O35" s="8"/>
+      <c r="P35" s="8"/>
+      <c r="Q35" s="7"/>
+      <c r="R35" s="7"/>
+      <c r="S35" s="7"/>
+      <c r="T35" s="7"/>
+      <c r="U35" s="7"/>
+      <c r="V35" s="8"/>
+      <c r="W35" s="8"/>
+      <c r="X35" s="8"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L19:L34" xr:uid="{28DE5D51-C321-4870-B1C8-48B479072D32}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L20:L35" xr:uid="{28DE5D51-C321-4870-B1C8-48B479072D32}">
       <formula1>"タスク,税,Spike,前提条件(技術的負債)"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="41" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="77" fitToHeight="0" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;F　&amp;A&amp;R&amp;D　&amp;T</oddHeader>
     <oddFooter>&amp;C&amp;P</oddFooter>
   </headerFooter>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="29" max="6" man="1"/>
+  </rowBreaks>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -2393,11 +2591,11 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="18.75"/>
   <cols>
-    <col min="1" max="1" width="2.58203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" style="3"/>
-    <col min="3" max="16384" width="8.6640625" style="1"/>
+    <col min="1" max="1" width="2.625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.625" style="3"/>
+    <col min="3" max="16384" width="8.625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4">
@@ -2646,68 +2844,102 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:L18"/>
+  <dimension ref="C2:M43"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="18.75"/>
   <cols>
-    <col min="1" max="1" width="2.58203125" style="1" customWidth="1"/>
-    <col min="2" max="8" width="8.6640625" style="1"/>
-    <col min="9" max="9" width="10.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.6640625" style="1"/>
+    <col min="1" max="1" width="2.625" style="1" customWidth="1"/>
+    <col min="2" max="9" width="8.625" style="1"/>
+    <col min="10" max="10" width="10.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="3:13">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:12">
-      <c r="B3" s="1" t="s">
+    <row r="3" spans="3:13">
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:12">
-      <c r="I12" s="1" t="s">
+    <row r="4" spans="3:13">
+      <c r="C4" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="3:13">
+      <c r="J13" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="2:12">
-      <c r="I14" s="1" t="s">
+    <row r="15" spans="3:13">
+      <c r="J15" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="K15" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="L14" s="1" t="s">
+      <c r="M15" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="2:12">
-      <c r="I15" s="1" t="s">
+    <row r="16" spans="3:13">
+      <c r="J16" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="2:12">
-      <c r="I16" s="1" t="s">
+    <row r="17" spans="10:11">
+      <c r="J17" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="9:10">
-      <c r="I18" s="4" t="s">
+    <row r="19" spans="10:11">
+      <c r="J19" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="K19" s="1" t="s">
         <v>54</v>
       </c>
+    </row>
+    <row r="41" spans="3:7">
+      <c r="C41" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="42" spans="3:7">
+      <c r="C42" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="D42" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="E42" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="F42" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="G42" s="16" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="43" spans="3:7">
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="80" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="74" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;F　&amp;A&amp;R&amp;D　&amp;T</oddHeader>
     <oddFooter>&amp;C&amp;P</oddFooter>
@@ -2724,10 +2956,10 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="18.75"/>
   <cols>
-    <col min="1" max="1" width="2.58203125" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.6640625" style="1"/>
+    <col min="1" max="1" width="2.625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:2">

</xml_diff>